<commit_message>
Subindo modelagem e script do banco de dados.
</commit_message>
<xml_diff>
--- a/Documentação/PlanilhadeGestão.xlsx
+++ b/Documentação/PlanilhadeGestão.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9acbaa33c33b352b/Área de Trabalho/SPTECH/P.I/1º Semestre/Projeto EA FC/Projeto-Individual-EAFC/Documentação/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9acbaa33c33b352b/Área de Trabalho/SPTECH/P.I/1º Semestre/Projeto EA FC/Projeto-Individual-FutStatsFC/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="303" documentId="8_{16A1973A-D8C0-485D-95AD-6B59008528A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F87B847-6E44-4A3A-853A-8BCFA30FDEB5}"/>
+  <xr:revisionPtr revIDLastSave="382" documentId="8_{16A1973A-D8C0-485D-95AD-6B59008528A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B18C98E-21D0-446F-9070-2B3BEDE22B74}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{45767E95-E26E-4D2A-B6B3-F481CCD0E30A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{45767E95-E26E-4D2A-B6B3-F481CCD0E30A}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Planilha de Riscos" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$A$2:$I$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$A$2:$I$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="123">
   <si>
     <t>ID</t>
   </si>
@@ -198,12 +198,6 @@
     <t>6.4</t>
   </si>
   <si>
-    <t>Sobre</t>
-  </si>
-  <si>
-    <t>6.5</t>
-  </si>
-  <si>
     <t>Dashboard</t>
   </si>
   <si>
@@ -225,9 +219,6 @@
     <t>7.4</t>
   </si>
   <si>
-    <t>7.5</t>
-  </si>
-  <si>
     <t>Máquina Virtual</t>
   </si>
   <si>
@@ -424,6 +415,33 @@
   </si>
   <si>
     <t>Revisar apresentação de todo o projeto.</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
+  </si>
+  <si>
+    <t>Prototipação da página de cadastro para acessar as dashboards.</t>
+  </si>
+  <si>
+    <t>Prototipação da página inicial do site.</t>
+  </si>
+  <si>
+    <t>Prototipação da tela de login para acessar as dashboards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipação das Dashboards. </t>
+  </si>
+  <si>
+    <t>Desenvolver página de cadastro para acessar as dashboards.</t>
+  </si>
+  <si>
+    <t>Desenvolver página inicial do site.</t>
+  </si>
+  <si>
+    <t>Desenvolver tela de login para acessar as dashboards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolver Dashboards. </t>
   </si>
 </sst>
 </file>
@@ -596,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -616,15 +634,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -636,6 +650,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -655,9 +675,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,16 +871,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>263</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>91</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>78</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>39</c:v>
@@ -937,10 +954,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1755,6 +1775,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
 <rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <global>
@@ -2141,24 +2165,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FC6B23-1C71-4B7B-81CF-524CE4FE0C8A}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>8</v>
       </c>
@@ -2173,7 +2197,7 @@
       <c r="H1" s="15"/>
       <c r="I1" s="16"/>
     </row>
-    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2196,13 +2220,13 @@
         <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -2213,10 +2237,10 @@
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F3" s="4">
         <v>5</v>
@@ -2225,13 +2249,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -2242,10 +2266,10 @@
         <v>17</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F4" s="4">
         <v>5</v>
@@ -2254,13 +2278,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -2271,10 +2295,10 @@
         <v>20</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F5" s="4">
         <v>5</v>
@@ -2283,13 +2307,13 @@
         <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -2300,10 +2324,10 @@
         <v>23</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F6" s="4">
         <v>5</v>
@@ -2312,13 +2336,13 @@
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -2329,10 +2353,10 @@
         <v>16</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F7" s="4">
         <v>5</v>
@@ -2341,13 +2365,13 @@
         <v>1</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>2</v>
       </c>
@@ -2358,10 +2382,10 @@
         <v>25</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
@@ -2370,13 +2394,13 @@
         <v>1</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>3</v>
       </c>
@@ -2387,10 +2411,10 @@
         <v>26</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="F9" s="4">
         <v>3</v>
@@ -2399,13 +2423,13 @@
         <v>1</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>4</v>
       </c>
@@ -2416,10 +2440,10 @@
         <v>29</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F10" s="4">
         <v>8</v>
@@ -2431,10 +2455,10 @@
         <v>9</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>5</v>
       </c>
@@ -2445,10 +2469,10 @@
         <v>31</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F11" s="4">
         <v>5</v>
@@ -2460,10 +2484,10 @@
         <v>9</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>6</v>
       </c>
@@ -2474,10 +2498,10 @@
         <v>33</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F12" s="4">
         <v>13</v>
@@ -2489,22 +2513,24 @@
         <v>9</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="D13" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F13" s="4">
         <v>13</v>
@@ -2516,22 +2542,24 @@
         <v>9</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D14" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F14" s="4">
         <v>13</v>
@@ -2543,22 +2571,24 @@
         <v>9</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>117</v>
+      </c>
       <c r="D15" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F15" s="4">
         <v>13</v>
@@ -2570,22 +2600,24 @@
         <v>9</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>118</v>
+      </c>
       <c r="D16" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F16" s="4">
         <v>13</v>
@@ -2597,22 +2629,24 @@
         <v>9</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>7</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="5"/>
       <c r="D17" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F17" s="4">
         <v>13</v>
@@ -2621,27 +2655,27 @@
         <v>1</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
-        <v>7</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F18" s="4">
         <v>13</v>
@@ -2650,25 +2684,27 @@
         <v>1</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="D19" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F19" s="4">
         <v>13</v>
@@ -2677,25 +2713,27 @@
         <v>1</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="D20" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F20" s="4">
         <v>13</v>
@@ -2704,25 +2742,27 @@
         <v>1</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>122</v>
+      </c>
       <c r="D21" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F21" s="4">
         <v>13</v>
@@ -2731,139 +2771,143 @@
         <v>1</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I21" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>8</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="F22" s="4">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G22" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I22" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>9</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="F23" s="4">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G23" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
-        <v>8</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>67</v>
       </c>
       <c r="F24" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G24" s="4">
         <v>2</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="I24" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
-        <v>9</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="F25" s="4">
         <v>5</v>
       </c>
       <c r="G25" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I25" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="E26" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F26" s="4">
         <v>8</v>
@@ -2872,183 +2916,125 @@
         <v>2</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>10</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="4">
+        <v>13</v>
+      </c>
+      <c r="G27" s="4">
+        <v>3</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="4">
+        <v>13</v>
+      </c>
+      <c r="G28" s="4">
+        <v>3</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="4">
         <v>8</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="4">
-        <v>5</v>
-      </c>
-      <c r="G27" s="4">
-        <v>1</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="4">
-        <v>8</v>
-      </c>
-      <c r="G28" s="4">
-        <v>2</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="4">
-        <v>10</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F29" s="4">
-        <v>13</v>
       </c>
       <c r="G29" s="4">
         <v>3</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F30" s="4">
-        <v>13</v>
-      </c>
-      <c r="G30" s="4">
-        <v>3</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F31" s="4">
-        <v>8</v>
-      </c>
-      <c r="G31" s="4">
-        <v>3</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I31" xr:uid="{53FC6B23-1C71-4B7B-81CF-524CE4FE0C8A}"/>
+  <autoFilter ref="A2:I29" xr:uid="{53FC6B23-1C71-4B7B-81CF-524CE4FE0C8A}"/>
   <mergeCells count="2">
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A1:F1"/>
   </mergeCells>
-  <conditionalFormatting sqref="D3:D31">
+  <conditionalFormatting sqref="D3:D29">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"Desejável"</formula>
     </cfRule>
@@ -3059,7 +3045,7 @@
       <formula>"Essencial"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I31">
+  <conditionalFormatting sqref="I3:I29">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Não iniciada"</formula>
     </cfRule>
@@ -3079,139 +3065,141 @@
   <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
-      <c r="F1" s="10" t="e" vm="1">
+      <c r="F1" s="14" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:6" ht="85.5" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="12" t="s">
+    </row>
+    <row r="3" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="14" t="s">
+      <c r="C3" s="7">
+        <f>SUM(C4:C8)</f>
+        <v>237</v>
+      </c>
+      <c r="D3" s="8">
+        <f>SUM(D4:D8)</f>
+        <v>237</v>
+      </c>
+      <c r="E3" s="8">
+        <f>SUM(E4:E8)</f>
+        <v>86</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3-E3</f>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="7">
+        <v>55</v>
+      </c>
+      <c r="D4" s="8">
+        <v>55</v>
+      </c>
+      <c r="E4" s="8">
+        <v>55</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" ref="F4:F8" si="0">D4-E4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7">
+        <v>78</v>
+      </c>
+      <c r="D5" s="8">
+        <v>78</v>
+      </c>
+      <c r="E5" s="8">
+        <v>31</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
+      <c r="C6" s="7">
+        <v>65</v>
+      </c>
+      <c r="D6" s="8">
+        <v>65</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="8">
-        <f>SUM(C4:C8)</f>
-        <v>263</v>
-      </c>
-      <c r="D3" s="9">
-        <f>SUM(D4:D8)</f>
-        <v>263</v>
-      </c>
-      <c r="E3" s="9">
-        <f>SUM(E4:E8)</f>
-        <v>30</v>
-      </c>
-      <c r="F3" s="9">
-        <f>D3-E3</f>
-        <v>233</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="8">
-        <v>55</v>
-      </c>
-      <c r="D4" s="9">
-        <v>55</v>
-      </c>
-      <c r="E4" s="9">
-        <v>30</v>
-      </c>
-      <c r="F4" s="9">
-        <f t="shared" ref="F4:F8" si="0">D4-E4</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="8">
-        <v>91</v>
-      </c>
-      <c r="D5" s="9">
-        <v>91</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9">
-        <f t="shared" si="0"/>
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="8">
-        <v>78</v>
-      </c>
-      <c r="D6" s="9">
-        <v>78</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9">
-        <f t="shared" si="0"/>
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>39</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>39</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9">
+      <c r="E7" s="8"/>
+      <c r="F7" s="8">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9">
+    <row r="8" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3231,21 +3219,21 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" customWidth="1"/>
-    <col min="8" max="8" width="77.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="77.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="118.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="118.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
@@ -3257,212 +3245,212 @@
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
     </row>
-    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="D3" s="13">
+        <v>2</v>
+      </c>
+      <c r="E3" s="13">
+        <v>3</v>
+      </c>
+      <c r="F3" s="13">
+        <v>6</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="21">
+      <c r="C4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="13">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="E4" s="13">
+        <v>3</v>
+      </c>
+      <c r="F4" s="13">
+        <v>3</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="21">
+      <c r="H4" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="13">
+        <v>1</v>
+      </c>
+      <c r="E5" s="13">
+        <v>3</v>
+      </c>
+      <c r="F5" s="13">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="13">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13">
         <v>2</v>
       </c>
-      <c r="E3" s="21">
+      <c r="F6" s="13">
+        <v>2</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="13">
+        <v>1</v>
+      </c>
+      <c r="E7" s="13">
         <v>3</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F7" s="13">
+        <v>3</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="B8" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="13">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <v>3</v>
+      </c>
+      <c r="F8" s="13">
+        <v>3</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="21">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="21">
+      <c r="D9" s="13">
         <v>1</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E9" s="13">
         <v>3</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F9" s="13">
         <v>3</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="21">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="21">
-        <v>1</v>
-      </c>
-      <c r="E5" s="21">
-        <v>3</v>
-      </c>
-      <c r="F5" s="21">
-        <v>3</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="21">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" s="21">
-        <v>1</v>
-      </c>
-      <c r="E6" s="21">
-        <v>2</v>
-      </c>
-      <c r="F6" s="21">
-        <v>2</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H6" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A7" s="21">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="21">
-        <v>1</v>
-      </c>
-      <c r="E7" s="21">
-        <v>3</v>
-      </c>
-      <c r="F7" s="21">
-        <v>3</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="21">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="21">
-        <v>1</v>
-      </c>
-      <c r="E8" s="21">
-        <v>3</v>
-      </c>
-      <c r="F8" s="21">
-        <v>3</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="21">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="21">
-        <v>1</v>
-      </c>
-      <c r="E9" s="21">
-        <v>3</v>
-      </c>
-      <c r="F9" s="21">
-        <v>3</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Subindo arquivos da API com cadastro e login integrados ao banco de dados.
</commit_message>
<xml_diff>
--- a/Documentação/PlanilhadeGestão.xlsx
+++ b/Documentação/PlanilhadeGestão.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9acbaa33c33b352b/Área de Trabalho/SPTECH/P.I/1º Semestre/Projeto EA FC/Projeto-Individual-FutStatsFC/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="382" documentId="8_{16A1973A-D8C0-485D-95AD-6B59008528A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B18C98E-21D0-446F-9070-2B3BEDE22B74}"/>
+  <xr:revisionPtr revIDLastSave="387" documentId="8_{16A1973A-D8C0-485D-95AD-6B59008528A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{297231C9-0259-4D9C-B06C-9F44264FB392}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{45767E95-E26E-4D2A-B6B3-F481CCD0E30A}"/>
   </bookViews>
@@ -441,7 +441,7 @@
     <t>Desenvolver tela de login para acessar as dashboards</t>
   </si>
   <si>
-    <t xml:space="preserve">Desenvolver Dashboards. </t>
+    <t xml:space="preserve">Desenvolver Dashboard. </t>
   </si>
 </sst>
 </file>
@@ -954,13 +954,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>86</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2167,8 +2167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FC6B23-1C71-4B7B-81CF-524CE4FE0C8A}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2571,7 +2571,7 @@
         <v>9</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2600,7 +2600,7 @@
         <v>9</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2629,7 +2629,7 @@
         <v>9</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3117,11 +3117,11 @@
       </c>
       <c r="E3" s="8">
         <f>SUM(E4:E8)</f>
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="F3" s="8">
         <f>D3-E3</f>
-        <v>151</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
@@ -3153,11 +3153,11 @@
         <v>78</v>
       </c>
       <c r="E5" s="8">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="F5" s="8">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Subindo tela Registrar Partida finalizada.
</commit_message>
<xml_diff>
--- a/Documentação/PlanilhadeGestão.xlsx
+++ b/Documentação/PlanilhadeGestão.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9acbaa33c33b352b/Área de Trabalho/SPTECH/P.I/1º Semestre/Projeto EA FC/Projeto-Individual-FutStatsFC/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="387" documentId="8_{16A1973A-D8C0-485D-95AD-6B59008528A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{297231C9-0259-4D9C-B06C-9F44264FB392}"/>
+  <xr:revisionPtr revIDLastSave="426" documentId="8_{16A1973A-D8C0-485D-95AD-6B59008528A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19232D67-2517-4A74-B9FC-655F7AF9B2B7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{45767E95-E26E-4D2A-B6B3-F481CCD0E30A}"/>
   </bookViews>
@@ -417,31 +417,31 @@
     <t>Revisar apresentação de todo o projeto.</t>
   </si>
   <si>
+    <t>Prototipação da página de cadastro para acessar as dashboards.</t>
+  </si>
+  <si>
+    <t>Prototipação da página inicial do site.</t>
+  </si>
+  <si>
+    <t>Prototipação da tela de login para acessar as dashboards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipação das Dashboards. </t>
+  </si>
+  <si>
+    <t>Desenvolver página de cadastro para acessar as dashboards.</t>
+  </si>
+  <si>
+    <t>Desenvolver página inicial do site.</t>
+  </si>
+  <si>
+    <t>Desenvolver tela de login para acessar as dashboards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolver Dashboard. </t>
+  </si>
+  <si>
     <t>Em andamento</t>
-  </si>
-  <si>
-    <t>Prototipação da página de cadastro para acessar as dashboards.</t>
-  </si>
-  <si>
-    <t>Prototipação da página inicial do site.</t>
-  </si>
-  <si>
-    <t>Prototipação da tela de login para acessar as dashboards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prototipação das Dashboards. </t>
-  </si>
-  <si>
-    <t>Desenvolver página de cadastro para acessar as dashboards.</t>
-  </si>
-  <si>
-    <t>Desenvolver página inicial do site.</t>
-  </si>
-  <si>
-    <t>Desenvolver tela de login para acessar as dashboards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desenvolver Dashboard. </t>
   </si>
 </sst>
 </file>
@@ -866,24 +866,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BurnDown!$D$3:$D$8</c:f>
+              <c:f>BurnDown!$E$3:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>237</c:v>
+                  <c:v>177</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>39</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -895,6 +889,22 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1088390736"/>
+        <c:axId val="1088392176"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -949,18 +959,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BurnDown!$E$3:$E$8</c:f>
+              <c:f>BurnDown!$D$3:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>112</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57</c:v>
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -980,9 +996,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1088390736"/>
-        <c:axId val="1088392176"/>
+        <c:axId val="384557839"/>
+        <c:axId val="699148255"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1088390736"/>
@@ -1091,6 +1108,66 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="699148255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="384557839"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="384557839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="699148255"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1775,10 +1852,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
 <rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <global>
@@ -2167,8 +2240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FC6B23-1C71-4B7B-81CF-524CE4FE0C8A}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2513,7 +2586,7 @@
         <v>9</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>114</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2524,7 +2597,7 @@
         <v>35</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>62</v>
@@ -2553,7 +2626,7 @@
         <v>37</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>62</v>
@@ -2582,7 +2655,7 @@
         <v>39</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>62</v>
@@ -2611,7 +2684,7 @@
         <v>41</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>62</v>
@@ -2629,7 +2702,7 @@
         <v>9</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>114</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2658,7 +2731,7 @@
         <v>76</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2669,7 +2742,7 @@
         <v>35</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>62</v>
@@ -2687,7 +2760,7 @@
         <v>76</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2698,7 +2771,7 @@
         <v>37</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>62</v>
@@ -2716,7 +2789,7 @@
         <v>76</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2727,7 +2800,7 @@
         <v>39</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>62</v>
@@ -2745,7 +2818,7 @@
         <v>76</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2756,7 +2829,7 @@
         <v>41</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>62</v>
@@ -2774,7 +2847,7 @@
         <v>76</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -3065,7 +3138,7 @@
   <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3112,16 +3185,16 @@
         <v>237</v>
       </c>
       <c r="D3" s="8">
-        <f>SUM(D4:D8)</f>
+        <f t="shared" ref="D3:D5" si="0">IF(E2&gt;D2,C3-(E2-D2),C3)</f>
         <v>237</v>
       </c>
       <c r="E3" s="8">
         <f>SUM(E4:E8)</f>
-        <v>112</v>
+        <v>177</v>
       </c>
       <c r="F3" s="8">
-        <f>D3-E3</f>
-        <v>125</v>
+        <f>IF((D3-E3) &lt; 0, 0, D3-E3)</f>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
@@ -3132,13 +3205,14 @@
         <v>55</v>
       </c>
       <c r="D4" s="8">
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="E4" s="8">
         <v>55</v>
       </c>
       <c r="F4" s="8">
-        <f t="shared" ref="F4:F8" si="0">D4-E4</f>
+        <f t="shared" ref="F4" si="1">IF((D4-E4) &lt; 0, 0, D4-E4)</f>
         <v>0</v>
       </c>
     </row>
@@ -3150,14 +3224,15 @@
         <v>78</v>
       </c>
       <c r="D5" s="8">
+        <f t="shared" si="0"/>
         <v>78</v>
       </c>
       <c r="E5" s="8">
-        <v>57</v>
+        <v>122</v>
       </c>
       <c r="F5" s="8">
-        <f t="shared" si="0"/>
-        <v>21</v>
+        <f>IF((D5-E5) &lt; 0, 0, D5-E5)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
@@ -3168,12 +3243,13 @@
         <v>65</v>
       </c>
       <c r="D6" s="8">
-        <v>65</v>
+        <f>IF(E5&gt;D5,C6-(E5-D5),C6)+5</f>
+        <v>26</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8">
-        <f t="shared" si="0"/>
-        <v>65</v>
+        <f t="shared" ref="F6:F8" si="2">IF((D6-E6) &lt; 0, 0, D6-E6)</f>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
@@ -3184,12 +3260,13 @@
         <v>39</v>
       </c>
       <c r="D7" s="8">
-        <v>39</v>
+        <f>IF(E6&gt;D6,C7-(E6-D6),C7) -5</f>
+        <v>34</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <f t="shared" si="2"/>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
@@ -3200,7 +3277,7 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3209,6 +3286,9 @@
     <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <ignoredErrors>
+    <ignoredError sqref="D3" formula="1"/>
+  </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -3219,7 +3299,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3230,7 +3310,7 @@
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="77.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="87.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="118.9" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Atualizando documentação e README
</commit_message>
<xml_diff>
--- a/Documentação/PlanilhadeGestão.xlsx
+++ b/Documentação/PlanilhadeGestão.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9acbaa33c33b352b/Área de Trabalho/SPTECH/P.I/1º Semestre/Projeto EA FC/Projeto-Individual-FutStatsFC/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="426" documentId="8_{16A1973A-D8C0-485D-95AD-6B59008528A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19232D67-2517-4A74-B9FC-655F7AF9B2B7}"/>
+  <xr:revisionPtr revIDLastSave="438" documentId="8_{16A1973A-D8C0-485D-95AD-6B59008528A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC958A6B-65A6-4342-AE11-5F665B3CC8C5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{45767E95-E26E-4D2A-B6B3-F481CCD0E30A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{45767E95-E26E-4D2A-B6B3-F481CCD0E30A}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -300,9 +300,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Projeto EA FC</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -442,6 +439,9 @@
   </si>
   <si>
     <t>Em andamento</t>
+  </si>
+  <si>
+    <t>Projeto FutStatsFC</t>
   </si>
 </sst>
 </file>
@@ -806,6 +806,66 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Gráfico de BurnDown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> - Projeto FutStatsFC</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -871,13 +931,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>177</c:v>
+                  <c:v>203</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1852,6 +1915,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
 <rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <global>
@@ -2240,8 +2307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FC6B23-1C71-4B7B-81CF-524CE4FE0C8A}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F27:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2597,7 +2664,7 @@
         <v>35</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>62</v>
@@ -2626,7 +2693,7 @@
         <v>37</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>62</v>
@@ -2655,7 +2722,7 @@
         <v>39</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>62</v>
@@ -2684,7 +2751,7 @@
         <v>41</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>62</v>
@@ -2728,10 +2795,10 @@
         <v>1</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>122</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2742,7 +2809,7 @@
         <v>35</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>62</v>
@@ -2757,7 +2824,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>60</v>
@@ -2771,7 +2838,7 @@
         <v>37</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>62</v>
@@ -2786,7 +2853,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>60</v>
@@ -2800,7 +2867,7 @@
         <v>39</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>62</v>
@@ -2815,7 +2882,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>60</v>
@@ -2829,7 +2896,7 @@
         <v>41</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>62</v>
@@ -2844,10 +2911,10 @@
         <v>1</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>122</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -2873,7 +2940,7 @@
         <v>2</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>60</v>
@@ -3000,10 +3067,10 @@
         <v>10</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>62</v>
@@ -3018,21 +3085,21 @@
         <v>3</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>62</v>
@@ -3047,21 +3114,21 @@
         <v>3</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>113</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>62</v>
@@ -3076,7 +3143,7 @@
         <v>3</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>61</v>
@@ -3138,7 +3205,7 @@
   <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3152,7 +3219,7 @@
   <sheetData>
     <row r="1" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -3190,11 +3257,11 @@
       </c>
       <c r="E3" s="8">
         <f>SUM(E4:E8)</f>
-        <v>177</v>
+        <v>203</v>
       </c>
       <c r="F3" s="8">
         <f>IF((D3-E3) &lt; 0, 0, D3-E3)</f>
-        <v>60</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
@@ -3237,7 +3304,7 @@
     </row>
     <row r="6" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" s="7">
         <v>65</v>
@@ -3246,15 +3313,17 @@
         <f>IF(E5&gt;D5,C6-(E5-D5),C6)+5</f>
         <v>26</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="8">
+        <v>26</v>
+      </c>
       <c r="F6" s="8">
         <f t="shared" ref="F6:F8" si="2">IF((D6-E6) &lt; 0, 0, D6-E6)</f>
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="7">
         <v>39</v>
@@ -3271,7 +3340,7 @@
     </row>
     <row r="8" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
@@ -3297,7 +3366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF14893-A8BE-47A1-AC77-483115869C49}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
@@ -3327,28 +3396,28 @@
     </row>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3356,10 +3425,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="D3" s="13">
         <v>2</v>
@@ -3371,10 +3440,10 @@
         <v>6</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3382,10 +3451,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D4" s="13">
         <v>1</v>
@@ -3397,10 +3466,10 @@
         <v>3</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3408,10 +3477,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D5" s="13">
         <v>1</v>
@@ -3423,10 +3492,10 @@
         <v>3</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3434,10 +3503,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="D6" s="13">
         <v>1</v>
@@ -3449,10 +3518,10 @@
         <v>2</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3460,10 +3529,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="D7" s="13">
         <v>1</v>
@@ -3475,10 +3544,10 @@
         <v>3</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3486,7 +3555,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>51</v>
@@ -3501,10 +3570,10 @@
         <v>3</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3512,10 +3581,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D9" s="13">
         <v>1</v>
@@ -3527,10 +3596,10 @@
         <v>3</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Subindo últimos detalhes da estilização das páginas e documentação finalizada!
</commit_message>
<xml_diff>
--- a/Documentação/PlanilhadeGestão.xlsx
+++ b/Documentação/PlanilhadeGestão.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9acbaa33c33b352b/Área de Trabalho/SPTECH/P.I/1º Semestre/Projeto EA FC/Projeto-Individual-FutStatsFC/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="438" documentId="8_{16A1973A-D8C0-485D-95AD-6B59008528A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC958A6B-65A6-4342-AE11-5F665B3CC8C5}"/>
+  <xr:revisionPtr revIDLastSave="442" documentId="8_{16A1973A-D8C0-485D-95AD-6B59008528A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A98D01F0-B46E-4A14-8814-DFE0F51C6D70}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{45767E95-E26E-4D2A-B6B3-F481CCD0E30A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{45767E95-E26E-4D2A-B6B3-F481CCD0E30A}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="121">
   <si>
     <t>ID</t>
   </si>
@@ -258,9 +258,6 @@
     <t>Concluída</t>
   </si>
   <si>
-    <t>Não iniciada</t>
-  </si>
-  <si>
     <t>Essencial</t>
   </si>
   <si>
@@ -436,9 +433,6 @@
   </si>
   <si>
     <t xml:space="preserve">Desenvolver Dashboard. </t>
-  </si>
-  <si>
-    <t>Em andamento</t>
   </si>
   <si>
     <t>Projeto FutStatsFC</t>
@@ -931,7 +925,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>203</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>55</c:v>
@@ -941,6 +935,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1915,10 +1912,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
 <rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <global>
@@ -2307,8 +2300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FC6B23-1C71-4B7B-81CF-524CE4FE0C8A}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F27:F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2360,7 +2353,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>7</v>
@@ -2377,10 +2370,10 @@
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3" s="4">
         <v>5</v>
@@ -2389,7 +2382,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>60</v>
@@ -2406,10 +2399,10 @@
         <v>17</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F4" s="4">
         <v>5</v>
@@ -2418,7 +2411,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>60</v>
@@ -2435,10 +2428,10 @@
         <v>20</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F5" s="4">
         <v>5</v>
@@ -2447,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>60</v>
@@ -2464,10 +2457,10 @@
         <v>23</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F6" s="4">
         <v>5</v>
@@ -2476,7 +2469,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>60</v>
@@ -2493,10 +2486,10 @@
         <v>16</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F7" s="4">
         <v>5</v>
@@ -2505,7 +2498,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>60</v>
@@ -2522,10 +2515,10 @@
         <v>25</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
@@ -2534,7 +2527,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>60</v>
@@ -2551,10 +2544,10 @@
         <v>26</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" s="4">
         <v>3</v>
@@ -2563,7 +2556,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>60</v>
@@ -2580,10 +2573,10 @@
         <v>29</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F10" s="4">
         <v>8</v>
@@ -2609,10 +2602,10 @@
         <v>31</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F11" s="4">
         <v>5</v>
@@ -2638,10 +2631,10 @@
         <v>33</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F12" s="4">
         <v>13</v>
@@ -2664,13 +2657,13 @@
         <v>35</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F13" s="4">
         <v>13</v>
@@ -2693,13 +2686,13 @@
         <v>37</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F14" s="4">
         <v>13</v>
@@ -2722,13 +2715,13 @@
         <v>39</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F15" s="4">
         <v>13</v>
@@ -2751,13 +2744,13 @@
         <v>41</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F16" s="4">
         <v>13</v>
@@ -2783,10 +2776,10 @@
         <v>43</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F17" s="4">
         <v>13</v>
@@ -2795,7 +2788,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>60</v>
@@ -2809,13 +2802,13 @@
         <v>35</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F18" s="4">
         <v>13</v>
@@ -2824,7 +2817,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>60</v>
@@ -2838,13 +2831,13 @@
         <v>37</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F19" s="4">
         <v>13</v>
@@ -2853,7 +2846,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>60</v>
@@ -2867,13 +2860,13 @@
         <v>39</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F20" s="4">
         <v>13</v>
@@ -2882,7 +2875,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>60</v>
@@ -2896,13 +2889,13 @@
         <v>41</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F21" s="4">
         <v>13</v>
@@ -2911,7 +2904,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>60</v>
@@ -2928,10 +2921,10 @@
         <v>49</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F22" s="4">
         <v>5</v>
@@ -2940,7 +2933,7 @@
         <v>2</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>60</v>
@@ -2957,10 +2950,10 @@
         <v>50</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F23" s="4">
         <v>5</v>
@@ -2969,7 +2962,7 @@
         <v>2</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>60</v>
@@ -2986,10 +2979,10 @@
         <v>54</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F24" s="4">
         <v>8</v>
@@ -2998,7 +2991,7 @@
         <v>2</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>60</v>
@@ -3015,10 +3008,10 @@
         <v>56</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F25" s="4">
         <v>5</v>
@@ -3027,7 +3020,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>60</v>
@@ -3044,10 +3037,10 @@
         <v>59</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F26" s="4">
         <v>8</v>
@@ -3056,7 +3049,7 @@
         <v>2</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>60</v>
@@ -3067,16 +3060,16 @@
         <v>10</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="D27" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F27" s="4">
         <v>13</v>
@@ -3085,27 +3078,27 @@
         <v>3</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>121</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>109</v>
-      </c>
       <c r="D28" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F28" s="4">
         <v>13</v>
@@ -3114,27 +3107,27 @@
         <v>3</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>121</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>112</v>
-      </c>
       <c r="D29" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F29" s="4">
         <v>8</v>
@@ -3143,10 +3136,10 @@
         <v>3</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -3205,7 +3198,7 @@
   <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3219,7 +3212,7 @@
   <sheetData>
     <row r="1" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -3231,21 +3224,21 @@
     <row r="2" spans="2:6" ht="85.5" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="7">
         <f>SUM(C4:C8)</f>
@@ -3257,16 +3250,16 @@
       </c>
       <c r="E3" s="8">
         <f>SUM(E4:E8)</f>
-        <v>203</v>
+        <v>237</v>
       </c>
       <c r="F3" s="8">
         <f>IF((D3-E3) &lt; 0, 0, D3-E3)</f>
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="7">
         <v>55</v>
@@ -3304,7 +3297,7 @@
     </row>
     <row r="6" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="7">
         <v>65</v>
@@ -3323,7 +3316,7 @@
     </row>
     <row r="7" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" s="7">
         <v>39</v>
@@ -3332,15 +3325,17 @@
         <f>IF(E6&gt;D6,C7-(E6-D6),C7) -5</f>
         <v>34</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="8">
+        <v>34</v>
+      </c>
       <c r="F7" s="8">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
@@ -3366,7 +3361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF14893-A8BE-47A1-AC77-483115869C49}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
@@ -3396,28 +3391,28 @@
     </row>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3425,10 +3420,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="D3" s="13">
         <v>2</v>
@@ -3440,10 +3435,10 @@
         <v>6</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3451,10 +3446,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="D4" s="13">
         <v>1</v>
@@ -3466,10 +3461,10 @@
         <v>3</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3477,10 +3472,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" s="13">
         <v>1</v>
@@ -3492,10 +3487,10 @@
         <v>3</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3503,10 +3498,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="D6" s="13">
         <v>1</v>
@@ -3518,10 +3513,10 @@
         <v>2</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3529,10 +3524,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="D7" s="13">
         <v>1</v>
@@ -3544,10 +3539,10 @@
         <v>3</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3555,7 +3550,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>51</v>
@@ -3570,10 +3565,10 @@
         <v>3</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3581,10 +3576,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D9" s="13">
         <v>1</v>
@@ -3596,10 +3591,10 @@
         <v>3</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>